<commit_message>
Updates for DOS review
</commit_message>
<xml_diff>
--- a/RapidMiner/NeuralNetHoldingFile.xlsx
+++ b/RapidMiner/NeuralNetHoldingFile.xlsx
@@ -124,7 +124,7 @@
         <v>8.28</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>10.351970226665214</v>
+        <v>8.182051697463905</v>
       </c>
     </row>
     <row r="3">
@@ -141,7 +141,7 @@
         <v>8.58</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>10.658496929317096</v>
+        <v>8.01007379356743</v>
       </c>
     </row>
     <row r="4">
@@ -158,7 +158,7 @@
         <v>8.29</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>10.39800675786884</v>
+        <v>8.797239129092313</v>
       </c>
     </row>
     <row r="5">
@@ -175,7 +175,7 @@
         <v>20.76</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>17.6526046466505</v>
+        <v>16.27321600439371</v>
       </c>
     </row>
     <row r="6">
@@ -192,7 +192,7 @@
         <v>12.06</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>9.745561633880184</v>
+        <v>8.066414953838478</v>
       </c>
     </row>
     <row r="7">
@@ -209,7 +209,7 @@
         <v>16.9</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>18.74515724943034</v>
+        <v>13.847952712232475</v>
       </c>
     </row>
     <row r="8">
@@ -226,7 +226,7 @@
         <v>8.12</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>9.745561633880184</v>
+        <v>8.066414953838478</v>
       </c>
     </row>
     <row r="9">
@@ -243,7 +243,7 @@
         <v>8.25</v>
       </c>
       <c r="E9" t="n" s="2">
-        <v>9.973073143711353</v>
+        <v>9.53112352006799</v>
       </c>
     </row>
     <row r="10">
@@ -260,7 +260,7 @@
         <v>27.85</v>
       </c>
       <c r="E10" t="n" s="2">
-        <v>24.333791323460595</v>
+        <v>24.439132215938336</v>
       </c>
     </row>
     <row r="11">
@@ -277,7 +277,7 @@
         <v>8.17</v>
       </c>
       <c r="E11" t="n" s="2">
-        <v>10.489829488419325</v>
+        <v>9.375665432811145</v>
       </c>
     </row>
     <row r="12">
@@ -294,7 +294,7 @@
         <v>8.17</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>11.964687563781217</v>
+        <v>9.509517250266017</v>
       </c>
     </row>
     <row r="13">
@@ -311,7 +311,7 @@
         <v>2.17</v>
       </c>
       <c r="E13" t="n" s="2">
-        <v>10.82677136057721</v>
+        <v>7.947518262177969</v>
       </c>
     </row>
     <row r="14">
@@ -328,7 +328,7 @@
         <v>1.09</v>
       </c>
       <c r="E14" t="n" s="2">
-        <v>6.137675518320698</v>
+        <v>1.6956331180355235</v>
       </c>
     </row>
     <row r="15">
@@ -345,7 +345,7 @@
         <v>1.09</v>
       </c>
       <c r="E15" t="n" s="2">
-        <v>20.596274871905443</v>
+        <v>26.72690099967158</v>
       </c>
     </row>
     <row r="16">
@@ -362,7 +362,7 @@
         <v>1.09</v>
       </c>
       <c r="E16" t="n" s="2">
-        <v>19.96752278541714</v>
+        <v>26.51960352917333</v>
       </c>
     </row>
     <row r="17">
@@ -379,7 +379,7 @@
         <v>1.09</v>
       </c>
       <c r="E17" t="n" s="2">
-        <v>4.274709272357068</v>
+        <v>1.888714214409287</v>
       </c>
     </row>
     <row r="18">
@@ -396,7 +396,7 @@
         <v>1.09</v>
       </c>
       <c r="E18" t="n" s="2">
-        <v>4.355130018351748</v>
+        <v>2.1161179869524958</v>
       </c>
     </row>
     <row r="19">
@@ -413,7 +413,7 @@
         <v>1.09</v>
       </c>
       <c r="E19" t="n" s="2">
-        <v>4.574996637445125</v>
+        <v>2.388644328245281</v>
       </c>
     </row>
     <row r="20">
@@ -430,7 +430,7 @@
         <v>6.87</v>
       </c>
       <c r="E20" t="n" s="2">
-        <v>4.744682643438207</v>
+        <v>2.532934269248223</v>
       </c>
     </row>
     <row r="21">
@@ -447,7 +447,7 @@
         <v>20.46</v>
       </c>
       <c r="E21" t="n" s="2">
-        <v>20.31326294004564</v>
+        <v>19.02960499761069</v>
       </c>
     </row>
     <row r="22">
@@ -464,7 +464,7 @@
         <v>8.06</v>
       </c>
       <c r="E22" t="n" s="2">
-        <v>10.145659147144983</v>
+        <v>10.320341398529736</v>
       </c>
     </row>
     <row r="23">
@@ -481,7 +481,7 @@
         <v>20.73</v>
       </c>
       <c r="E23" t="n" s="2">
-        <v>18.039799380735218</v>
+        <v>18.820685716437655</v>
       </c>
     </row>
     <row r="24">
@@ -498,7 +498,7 @@
         <v>1.17</v>
       </c>
       <c r="E24" t="n" s="2">
-        <v>3.885061722960902</v>
+        <v>0.02506131343921325</v>
       </c>
     </row>
     <row r="25">
@@ -515,7 +515,7 @@
         <v>1.14</v>
       </c>
       <c r="E25" t="n" s="2">
-        <v>0.5918503432865094</v>
+        <v>1.1374866008016582</v>
       </c>
     </row>
     <row r="26">
@@ -532,7 +532,7 @@
         <v>2.17</v>
       </c>
       <c r="E26" t="n" s="2">
-        <v>5.403786876811669</v>
+        <v>2.4715826355868273</v>
       </c>
     </row>
     <row r="27">
@@ -549,7 +549,7 @@
         <v>20.41</v>
       </c>
       <c r="E27" t="n" s="2">
-        <v>21.181651408808204</v>
+        <v>19.665250046680914</v>
       </c>
     </row>
     <row r="28">
@@ -566,7 +566,7 @@
         <v>8.15</v>
       </c>
       <c r="E28" t="n" s="2">
-        <v>9.394385310081635</v>
+        <v>7.830657864141614</v>
       </c>
     </row>
     <row r="29">
@@ -583,7 +583,7 @@
         <v>20.46</v>
       </c>
       <c r="E29" t="n" s="2">
-        <v>11.769280849023211</v>
+        <v>10.025872472929654</v>
       </c>
     </row>
     <row r="30">
@@ -600,7 +600,7 @@
         <v>20.45</v>
       </c>
       <c r="E30" t="n" s="2">
-        <v>22.163637085763483</v>
+        <v>20.72044788298934</v>
       </c>
     </row>
     <row r="31">
@@ -617,7 +617,7 @@
         <v>8.14</v>
       </c>
       <c r="E31" t="n" s="2">
-        <v>9.16258801986213</v>
+        <v>7.314630481657307</v>
       </c>
     </row>
     <row r="32">
@@ -634,7 +634,7 @@
         <v>11.86</v>
       </c>
       <c r="E32" t="n" s="2">
-        <v>17.420382517786653</v>
+        <v>16.286917622833272</v>
       </c>
     </row>
     <row r="33">
@@ -651,7 +651,7 @@
         <v>20.76</v>
       </c>
       <c r="E33" t="n" s="2">
-        <v>22.29816361431771</v>
+        <v>21.475218246340425</v>
       </c>
     </row>
     <row r="34">
@@ -668,7 +668,7 @@
         <v>8.23</v>
       </c>
       <c r="E34" t="n" s="2">
-        <v>10.657450261948675</v>
+        <v>8.243427696238571</v>
       </c>
     </row>
     <row r="35">
@@ -685,7 +685,7 @@
         <v>8.18</v>
       </c>
       <c r="E35" t="n" s="2">
-        <v>9.564698512444036</v>
+        <v>8.373913822829692</v>
       </c>
     </row>
     <row r="36">
@@ -702,7 +702,7 @@
         <v>8.03</v>
       </c>
       <c r="E36" t="n" s="2">
-        <v>10.346375450285333</v>
+        <v>8.106373956737517</v>
       </c>
     </row>
     <row r="37">
@@ -719,7 +719,7 @@
         <v>8.14</v>
       </c>
       <c r="E37" t="n" s="2">
-        <v>10.783599387787328</v>
+        <v>8.055778489858271</v>
       </c>
     </row>
     <row r="38">
@@ -736,7 +736,7 @@
         <v>8.14</v>
       </c>
       <c r="E38" t="n" s="2">
-        <v>10.297907016581076</v>
+        <v>8.72494440346205</v>
       </c>
     </row>
     <row r="39">
@@ -753,7 +753,7 @@
         <v>8.1</v>
       </c>
       <c r="E39" t="n" s="2">
-        <v>10.266547679756329</v>
+        <v>8.116633350158384</v>
       </c>
     </row>
     <row r="40">
@@ -770,7 +770,7 @@
         <v>8.16</v>
       </c>
       <c r="E40" t="n" s="2">
-        <v>8.69664008749861</v>
+        <v>7.306611216007376</v>
       </c>
     </row>
     <row r="41">
@@ -787,7 +787,7 @@
         <v>20.8</v>
       </c>
       <c r="E41" t="n" s="2">
-        <v>20.967364435325578</v>
+        <v>18.484776081815134</v>
       </c>
     </row>
     <row r="42">
@@ -804,7 +804,7 @@
         <v>12.44</v>
       </c>
       <c r="E42" t="n" s="2">
-        <v>18.01536424678517</v>
+        <v>14.592042015506177</v>
       </c>
     </row>
     <row r="43">
@@ -821,7 +821,7 @@
         <v>14.87</v>
       </c>
       <c r="E43" t="n" s="2">
-        <v>8.469087234507889</v>
+        <v>9.408867436975976</v>
       </c>
     </row>
     <row r="44">
@@ -838,7 +838,7 @@
         <v>7.97</v>
       </c>
       <c r="E44" t="n" s="2">
-        <v>10.139324813307761</v>
+        <v>10.193821861256627</v>
       </c>
     </row>
     <row r="45">
@@ -855,7 +855,7 @@
         <v>8.03</v>
       </c>
       <c r="E45" t="n" s="2">
-        <v>10.19380039210558</v>
+        <v>10.407324039797578</v>
       </c>
     </row>
     <row r="46">
@@ -872,7 +872,7 @@
         <v>7.99</v>
       </c>
       <c r="E46" t="n" s="2">
-        <v>8.22488392000299</v>
+        <v>9.58022861008955</v>
       </c>
     </row>
     <row r="47">
@@ -889,7 +889,7 @@
         <v>7.97</v>
       </c>
       <c r="E47" t="n" s="2">
-        <v>9.933512019428596</v>
+        <v>9.2356417145884</v>
       </c>
     </row>
     <row r="48">
@@ -906,7 +906,7 @@
         <v>7.92</v>
       </c>
       <c r="E48" t="n" s="2">
-        <v>10.239969069288648</v>
+        <v>8.82987739958533</v>
       </c>
     </row>
     <row r="49">
@@ -923,7 +923,7 @@
         <v>8.09</v>
       </c>
       <c r="E49" t="n" s="2">
-        <v>10.218629746411859</v>
+        <v>10.536044417889133</v>
       </c>
     </row>
     <row r="50">
@@ -940,7 +940,7 @@
         <v>10.3</v>
       </c>
       <c r="E50" t="n" s="2">
-        <v>9.640317481094591</v>
+        <v>8.061966418738706</v>
       </c>
     </row>
     <row r="51">
@@ -957,7 +957,7 @@
         <v>20.62</v>
       </c>
       <c r="E51" t="n" s="2">
-        <v>22.145368892379715</v>
+        <v>20.182618982373334</v>
       </c>
     </row>
     <row r="52">
@@ -974,7 +974,7 @@
         <v>9.05</v>
       </c>
       <c r="E52" t="n" s="2">
-        <v>10.086533950943624</v>
+        <v>8.53929672348277</v>
       </c>
     </row>
     <row r="53">
@@ -991,7 +991,7 @@
         <v>7.13</v>
       </c>
       <c r="E53" t="n" s="2">
-        <v>9.029931304587366</v>
+        <v>8.045665895994912</v>
       </c>
     </row>
     <row r="54">
@@ -1008,7 +1008,7 @@
         <v>2.55</v>
       </c>
       <c r="E54" t="n" s="2">
-        <v>10.098329299261668</v>
+        <v>8.712526974050162</v>
       </c>
     </row>
     <row r="55">
@@ -1025,7 +1025,7 @@
         <v>8.23</v>
       </c>
       <c r="E55" t="n" s="2">
-        <v>5.608300884084443</v>
+        <v>7.143281865265328</v>
       </c>
     </row>
     <row r="56">
@@ -1042,7 +1042,7 @@
         <v>8.16</v>
       </c>
       <c r="E56" t="n" s="2">
-        <v>10.07703985676082</v>
+        <v>7.9735520826985145</v>
       </c>
     </row>
     <row r="57">
@@ -1059,7 +1059,7 @@
         <v>8.18</v>
       </c>
       <c r="E57" t="n" s="2">
-        <v>9.309621788199465</v>
+        <v>8.116408979950942</v>
       </c>
     </row>
     <row r="58">
@@ -1076,7 +1076,7 @@
         <v>8.18</v>
       </c>
       <c r="E58" t="n" s="2">
-        <v>9.255178700658595</v>
+        <v>8.126672533600978</v>
       </c>
     </row>
     <row r="59">
@@ -1093,7 +1093,7 @@
         <v>8.13</v>
       </c>
       <c r="E59" t="n" s="2">
-        <v>9.928592934043733</v>
+        <v>8.205673189421052</v>
       </c>
     </row>
     <row r="60">
@@ -1110,7 +1110,7 @@
         <v>8.15</v>
       </c>
       <c r="E60" t="n" s="2">
-        <v>9.090179306267204</v>
+        <v>8.113518481252118</v>
       </c>
     </row>
     <row r="61">
@@ -1127,7 +1127,7 @@
         <v>1.16</v>
       </c>
       <c r="E61" t="n" s="2">
-        <v>5.645079202059808</v>
+        <v>7.259661300889963</v>
       </c>
     </row>
     <row r="62">
@@ -1144,7 +1144,7 @@
         <v>10.69</v>
       </c>
       <c r="E62" t="n" s="2">
-        <v>7.766487207389776</v>
+        <v>5.665243484611729</v>
       </c>
     </row>
     <row r="63">
@@ -1161,7 +1161,7 @@
         <v>20.79</v>
       </c>
       <c r="E63" t="n" s="2">
-        <v>12.491346974508957</v>
+        <v>9.796931009270766</v>
       </c>
     </row>
     <row r="64">
@@ -1178,7 +1178,7 @@
         <v>8.17</v>
       </c>
       <c r="E64" t="n" s="2">
-        <v>4.436413892974617</v>
+        <v>8.55116233533741</v>
       </c>
     </row>
     <row r="65">
@@ -1195,7 +1195,7 @@
         <v>8.16</v>
       </c>
       <c r="E65" t="n" s="2">
-        <v>10.46483489039873</v>
+        <v>8.22340459814114</v>
       </c>
     </row>
     <row r="66">
@@ -1212,7 +1212,7 @@
         <v>8.22</v>
       </c>
       <c r="E66" t="n" s="2">
-        <v>9.977412322435855</v>
+        <v>8.19767477605039</v>
       </c>
     </row>
     <row r="67">
@@ -1229,7 +1229,7 @@
         <v>8.19</v>
       </c>
       <c r="E67" t="n" s="2">
-        <v>8.915695169299292</v>
+        <v>8.043622189151318</v>
       </c>
     </row>
     <row r="68">
@@ -1246,7 +1246,7 @@
         <v>8.11</v>
       </c>
       <c r="E68" t="n" s="2">
-        <v>8.78712410515608</v>
+        <v>8.041585393652957</v>
       </c>
     </row>
     <row r="69">
@@ -1263,7 +1263,7 @@
         <v>8.18</v>
       </c>
       <c r="E69" t="n" s="2">
-        <v>10.341518350022723</v>
+        <v>9.655701189819537</v>
       </c>
     </row>
     <row r="70">
@@ -1280,7 +1280,7 @@
         <v>8.2</v>
       </c>
       <c r="E70" t="n" s="2">
-        <v>8.962870350347295</v>
+        <v>8.124654988460366</v>
       </c>
     </row>
     <row r="71">
@@ -1297,7 +1297,7 @@
         <v>13.03</v>
       </c>
       <c r="E71" t="n" s="2">
-        <v>8.484181044225805</v>
+        <v>8.038089748485742</v>
       </c>
     </row>
     <row r="72">
@@ -1314,7 +1314,7 @@
         <v>8.4</v>
       </c>
       <c r="E72" t="n" s="2">
-        <v>6.806641010482284</v>
+        <v>9.295191874139414</v>
       </c>
     </row>
     <row r="73">
@@ -1331,7 +1331,7 @@
         <v>8.09</v>
       </c>
       <c r="E73" t="n" s="2">
-        <v>9.255178700658595</v>
+        <v>8.126672533600978</v>
       </c>
     </row>
     <row r="74">
@@ -1348,7 +1348,7 @@
         <v>8.31</v>
       </c>
       <c r="E74" t="n" s="2">
-        <v>10.252721014411817</v>
+        <v>8.279503628577823</v>
       </c>
     </row>
     <row r="75">
@@ -1365,7 +1365,7 @@
         <v>8.32</v>
       </c>
       <c r="E75" t="n" s="2">
-        <v>9.685985485221408</v>
+        <v>8.188415164548694</v>
       </c>
     </row>
     <row r="76">
@@ -1382,7 +1382,7 @@
         <v>8.33</v>
       </c>
       <c r="E76" t="n" s="2">
-        <v>9.66041225960461</v>
+        <v>8.064966541540802</v>
       </c>
     </row>
     <row r="77">
@@ -1399,7 +1399,7 @@
         <v>8.29</v>
       </c>
       <c r="E77" t="n" s="2">
-        <v>9.255178700658595</v>
+        <v>8.126672533600978</v>
       </c>
     </row>
     <row r="78">
@@ -1416,7 +1416,7 @@
         <v>8.3</v>
       </c>
       <c r="E78" t="n" s="2">
-        <v>8.78712410515608</v>
+        <v>8.041585393652957</v>
       </c>
     </row>
     <row r="79">
@@ -1433,7 +1433,7 @@
         <v>8.24</v>
       </c>
       <c r="E79" t="n" s="2">
-        <v>8.996024536094266</v>
+        <v>8.112797248765638</v>
       </c>
     </row>
     <row r="80">
@@ -1450,7 +1450,7 @@
         <v>8.23</v>
       </c>
       <c r="E80" t="n" s="2">
-        <v>10.311683321179174</v>
+        <v>9.158211014309318</v>
       </c>
     </row>
     <row r="81">
@@ -1467,7 +1467,7 @@
         <v>4.47</v>
       </c>
       <c r="E81" t="n" s="2">
-        <v>8.484181044225805</v>
+        <v>8.038089748485742</v>
       </c>
     </row>
     <row r="82">
@@ -1484,7 +1484,7 @@
         <v>2.52</v>
       </c>
       <c r="E82" t="n" s="2">
-        <v>3.2441943929912895</v>
+        <v>1.0771238161772523</v>
       </c>
     </row>
     <row r="83">
@@ -1501,7 +1501,7 @@
         <v>2.45</v>
       </c>
       <c r="E83" t="n" s="2">
-        <v>3.5435301702329305</v>
+        <v>1.4277459836095865</v>
       </c>
     </row>
     <row r="84">
@@ -1518,7 +1518,7 @@
         <v>20.85</v>
       </c>
       <c r="E84" t="n" s="2">
-        <v>23.456366921903626</v>
+        <v>26.764185565943876</v>
       </c>
     </row>
     <row r="85">
@@ -1535,7 +1535,7 @@
         <v>8.32</v>
       </c>
       <c r="E85" t="n" s="2">
-        <v>10.20869925621589</v>
+        <v>9.051311878931172</v>
       </c>
     </row>
     <row r="86">
@@ -1552,7 +1552,7 @@
         <v>8.26</v>
       </c>
       <c r="E86" t="n" s="2">
-        <v>8.002732348752657</v>
+        <v>7.960264118588261</v>
       </c>
     </row>
     <row r="87">
@@ -1569,7 +1569,7 @@
         <v>2.2</v>
       </c>
       <c r="E87" t="n" s="2">
-        <v>7.545007385241588</v>
+        <v>3.844910428363093</v>
       </c>
     </row>
     <row r="88">
@@ -1586,7 +1586,7 @@
         <v>1.49</v>
       </c>
       <c r="E88" t="n" s="2">
-        <v>5.385938882777005</v>
+        <v>2.8733073656649424</v>
       </c>
     </row>
     <row r="89">
@@ -1603,7 +1603,7 @@
         <v>1.56</v>
       </c>
       <c r="E89" t="n" s="2">
-        <v>7.0727015252951215</v>
+        <v>5.382038655670804</v>
       </c>
     </row>
     <row r="90">
@@ -1620,7 +1620,7 @@
         <v>1.52</v>
       </c>
       <c r="E90" t="n" s="2">
-        <v>8.526904725914775</v>
+        <v>7.221737408815704</v>
       </c>
     </row>
     <row r="91">
@@ -1637,7 +1637,7 @@
         <v>8.33</v>
       </c>
       <c r="E91" t="n" s="2">
-        <v>10.04112269108666</v>
+        <v>8.085485626565141</v>
       </c>
     </row>
     <row r="92">
@@ -1654,7 +1654,7 @@
         <v>2.56</v>
       </c>
       <c r="E92" t="n" s="2">
-        <v>9.999165545463077</v>
+        <v>7.833028805737936</v>
       </c>
     </row>
     <row r="93">
@@ -1671,7 +1671,7 @@
         <v>21.88</v>
       </c>
       <c r="E93" t="n" s="2">
-        <v>6.800314666574202</v>
+        <v>3.289320882033337</v>
       </c>
     </row>
     <row r="94">
@@ -1688,7 +1688,7 @@
         <v>8.31</v>
       </c>
       <c r="E94" t="n" s="2">
-        <v>10.363906796077329</v>
+        <v>10.369883126128844</v>
       </c>
     </row>
     <row r="95">
@@ -1705,7 +1705,7 @@
         <v>2.54</v>
       </c>
       <c r="E95" t="n" s="2">
-        <v>10.059979985531857</v>
+        <v>8.122221111596561</v>
       </c>
     </row>
     <row r="96">
@@ -1722,7 +1722,7 @@
         <v>1.47</v>
       </c>
       <c r="E96" t="n" s="2">
-        <v>5.754107968917101</v>
+        <v>2.489495835460122</v>
       </c>
     </row>
     <row r="97">
@@ -1739,7 +1739,7 @@
         <v>1.48</v>
       </c>
       <c r="E97" t="n" s="2">
-        <v>3.659338020570445</v>
+        <v>1.3219314005900458</v>
       </c>
     </row>
     <row r="98">
@@ -1756,7 +1756,7 @@
         <v>20.41</v>
       </c>
       <c r="E98" t="n" s="2">
-        <v>25.740674593698323</v>
+        <v>20.241808453629286</v>
       </c>
     </row>
     <row r="99">
@@ -1773,7 +1773,7 @@
         <v>20.77</v>
       </c>
       <c r="E99" t="n" s="2">
-        <v>23.278111487034188</v>
+        <v>22.6937769504415</v>
       </c>
     </row>
     <row r="100">
@@ -1790,7 +1790,7 @@
         <v>8.28</v>
       </c>
       <c r="E100" t="n" s="2">
-        <v>10.098329299261668</v>
+        <v>8.712526974050162</v>
       </c>
     </row>
     <row r="101">
@@ -1807,7 +1807,7 @@
         <v>8.21</v>
       </c>
       <c r="E101" t="n" s="2">
-        <v>8.682846499817288</v>
+        <v>8.04014545100684</v>
       </c>
     </row>
     <row r="102">
@@ -1824,7 +1824,7 @@
         <v>8.2</v>
       </c>
       <c r="E102" t="n" s="2">
-        <v>9.957962346397379</v>
+        <v>8.007724151425661</v>
       </c>
     </row>
     <row r="103">
@@ -1841,7 +1841,7 @@
         <v>8.23</v>
       </c>
       <c r="E103" t="n" s="2">
-        <v>9.914413492686155</v>
+        <v>7.770721672306273</v>
       </c>
     </row>
     <row r="104">
@@ -1858,7 +1858,7 @@
         <v>2.52</v>
       </c>
       <c r="E104" t="n" s="2">
-        <v>4.275141676283045</v>
+        <v>1.6398439401583076</v>
       </c>
     </row>
     <row r="105">
@@ -1875,7 +1875,7 @@
         <v>20.49</v>
       </c>
       <c r="E105" t="n" s="2">
-        <v>23.392397407221146</v>
+        <v>28.36344187304499</v>
       </c>
     </row>
     <row r="106">
@@ -1892,7 +1892,7 @@
         <v>8.14</v>
       </c>
       <c r="E106" t="n" s="2">
-        <v>9.948125914688914</v>
+        <v>7.558956891721355</v>
       </c>
     </row>
     <row r="107">
@@ -1909,7 +1909,7 @@
         <v>8.14</v>
       </c>
       <c r="E107" t="n" s="2">
-        <v>10.294394424849045</v>
+        <v>10.11188311612278</v>
       </c>
     </row>
     <row r="108">
@@ -1926,7 +1926,7 @@
         <v>8.16</v>
       </c>
       <c r="E108" t="n" s="2">
-        <v>10.048100530243811</v>
+        <v>8.414682326070128</v>
       </c>
     </row>
     <row r="109">
@@ -1943,7 +1943,7 @@
         <v>8.03</v>
       </c>
       <c r="E109" t="n" s="2">
-        <v>9.345182377042667</v>
+        <v>7.522058747309277</v>
       </c>
     </row>
     <row r="110">
@@ -1960,7 +1960,7 @@
         <v>16.72</v>
       </c>
       <c r="E110" t="n" s="2">
-        <v>21.676008169327673</v>
+        <v>20.68283916500375</v>
       </c>
     </row>
     <row r="111">
@@ -1977,7 +1977,7 @@
         <v>8.25</v>
       </c>
       <c r="E111" t="n" s="2">
-        <v>9.617526210171158</v>
+        <v>7.274747862484206</v>
       </c>
     </row>
     <row r="112">
@@ -1994,7 +1994,7 @@
         <v>8.24</v>
       </c>
       <c r="E112" t="n" s="2">
-        <v>8.392476465250423</v>
+        <v>7.491042587564012</v>
       </c>
     </row>
     <row r="113">
@@ -2011,7 +2011,7 @@
         <v>20.39</v>
       </c>
       <c r="E113" t="n" s="2">
-        <v>20.264709561320966</v>
+        <v>20.303155578657908</v>
       </c>
     </row>
     <row r="114">
@@ -2028,7 +2028,7 @@
         <v>8.23</v>
       </c>
       <c r="E114" t="n" s="2">
-        <v>9.213311233314693</v>
+        <v>8.499619843263137</v>
       </c>
     </row>
     <row r="115">
@@ -2045,7 +2045,7 @@
         <v>8.45</v>
       </c>
       <c r="E115" t="n" s="2">
-        <v>9.797931168002314</v>
+        <v>8.755481845386008</v>
       </c>
     </row>
     <row r="116">
@@ -2062,7 +2062,7 @@
         <v>20.03</v>
       </c>
       <c r="E116" t="n" s="2">
-        <v>19.620952432314656</v>
+        <v>20.213788819687792</v>
       </c>
     </row>
     <row r="117">
@@ -2079,7 +2079,7 @@
         <v>8.23</v>
       </c>
       <c r="E117" t="n" s="2">
-        <v>9.904997975992641</v>
+        <v>8.058327007554423</v>
       </c>
     </row>
     <row r="118">
@@ -2096,7 +2096,7 @@
         <v>14.1</v>
       </c>
       <c r="E118" t="n" s="2">
-        <v>10.218462980976643</v>
+        <v>9.180512015107126</v>
       </c>
     </row>
     <row r="119">
@@ -2113,7 +2113,7 @@
         <v>8.25</v>
       </c>
       <c r="E119" t="n" s="2">
-        <v>9.430325824776917</v>
+        <v>8.261527884331175</v>
       </c>
     </row>
     <row r="120">
@@ -2130,7 +2130,7 @@
         <v>23.73</v>
       </c>
       <c r="E120" t="n" s="2">
-        <v>18.95426485498121</v>
+        <v>19.902527532373288</v>
       </c>
     </row>
     <row r="121">
@@ -2147,7 +2147,7 @@
         <v>29.51</v>
       </c>
       <c r="E121" t="n" s="2">
-        <v>25.43466101131131</v>
+        <v>25.947419935982627</v>
       </c>
     </row>
     <row r="122">
@@ -2164,7 +2164,7 @@
         <v>8.3</v>
       </c>
       <c r="E122" t="n" s="2">
-        <v>12.552980186398933</v>
+        <v>12.56686531163366</v>
       </c>
     </row>
     <row r="123">
@@ -2181,7 +2181,7 @@
         <v>20.46</v>
       </c>
       <c r="E123" t="n" s="2">
-        <v>23.071368537550914</v>
+        <v>17.82183397456314</v>
       </c>
     </row>
     <row r="124">
@@ -2198,7 +2198,7 @@
         <v>20.74</v>
       </c>
       <c r="E124" t="n" s="2">
-        <v>24.404817955311735</v>
+        <v>21.542950261359646</v>
       </c>
     </row>
     <row r="125">
@@ -2215,7 +2215,7 @@
         <v>20.92</v>
       </c>
       <c r="E125" t="n" s="2">
-        <v>24.803123919381786</v>
+        <v>21.797556850170416</v>
       </c>
     </row>
     <row r="126">
@@ -2232,7 +2232,7 @@
         <v>8.31</v>
       </c>
       <c r="E126" t="n" s="2">
-        <v>17.493437299347335</v>
+        <v>-5.322175589390998</v>
       </c>
     </row>
     <row r="127">
@@ -2249,7 +2249,7 @@
         <v>20.42</v>
       </c>
       <c r="E127" t="n" s="2">
-        <v>22.010333672953927</v>
+        <v>19.325920804401452</v>
       </c>
     </row>
     <row r="128">
@@ -2266,7 +2266,7 @@
         <v>18.86</v>
       </c>
       <c r="E128" t="n" s="2">
-        <v>22.425316227693685</v>
+        <v>19.928636997784185</v>
       </c>
     </row>
     <row r="129">
@@ -2283,7 +2283,7 @@
         <v>20.68</v>
       </c>
       <c r="E129" t="n" s="2">
-        <v>21.78741032127838</v>
+        <v>19.706757154857623</v>
       </c>
     </row>
     <row r="130">
@@ -2300,7 +2300,7 @@
         <v>8.15</v>
       </c>
       <c r="E130" t="n" s="2">
-        <v>13.083448170016174</v>
+        <v>10.766543814641956</v>
       </c>
     </row>
     <row r="131">
@@ -2317,7 +2317,7 @@
         <v>8.13</v>
       </c>
       <c r="E131" t="n" s="2">
-        <v>9.740465670720338</v>
+        <v>8.672087666962952</v>
       </c>
     </row>
     <row r="132">
@@ -2334,7 +2334,7 @@
         <v>20.7</v>
       </c>
       <c r="E132" t="n" s="2">
-        <v>21.585070249176386</v>
+        <v>20.519673649038754</v>
       </c>
     </row>
     <row r="133">
@@ -2351,7 +2351,7 @@
         <v>8.04</v>
       </c>
       <c r="E133" t="n" s="2">
-        <v>8.655056050417905</v>
+        <v>6.238616055983375</v>
       </c>
     </row>
     <row r="134">
@@ -2368,7 +2368,7 @@
         <v>8.07</v>
       </c>
       <c r="E134" t="n" s="2">
-        <v>10.583540751308638</v>
+        <v>8.734476878105456</v>
       </c>
     </row>
     <row r="135">
@@ -2385,7 +2385,7 @@
         <v>8.04</v>
       </c>
       <c r="E135" t="n" s="2">
-        <v>13.380256726792942</v>
+        <v>10.600054037404046</v>
       </c>
     </row>
     <row r="136">
@@ -2402,7 +2402,7 @@
         <v>20.47</v>
       </c>
       <c r="E136" t="n" s="2">
-        <v>22.052030762651345</v>
+        <v>19.22901239798358</v>
       </c>
     </row>
     <row r="137">
@@ -2419,7 +2419,7 @@
         <v>20.61</v>
       </c>
       <c r="E137" t="n" s="2">
-        <v>21.037549862196396</v>
+        <v>19.7936017952748</v>
       </c>
     </row>
     <row r="138">
@@ -2436,7 +2436,7 @@
         <v>8.21</v>
       </c>
       <c r="E138" t="n" s="2">
-        <v>13.020322959910855</v>
+        <v>10.994586801409023</v>
       </c>
     </row>
     <row r="139">
@@ -2453,7 +2453,7 @@
         <v>8.18</v>
       </c>
       <c r="E139" t="n" s="2">
-        <v>11.323670952052478</v>
+        <v>8.95520482610032</v>
       </c>
     </row>
     <row r="140">
@@ -2470,7 +2470,7 @@
         <v>8.22</v>
       </c>
       <c r="E140" t="n" s="2">
-        <v>11.480609371828253</v>
+        <v>9.476101435602839</v>
       </c>
     </row>
     <row r="141">
@@ -2487,7 +2487,7 @@
         <v>8.13</v>
       </c>
       <c r="E141" t="n" s="2">
-        <v>9.333877624474454</v>
+        <v>8.480656440217233</v>
       </c>
     </row>
     <row r="142">
@@ -2504,7 +2504,7 @@
         <v>8.13</v>
       </c>
       <c r="E142" t="n" s="2">
-        <v>8.090504023327627</v>
+        <v>8.1101082688071</v>
       </c>
     </row>
     <row r="143">
@@ -2521,7 +2521,7 @@
         <v>8.17</v>
       </c>
       <c r="E143" t="n" s="2">
-        <v>9.84949112881635</v>
+        <v>8.042097232069027</v>
       </c>
     </row>
     <row r="144">
@@ -2538,7 +2538,7 @@
         <v>8.14</v>
       </c>
       <c r="E144" t="n" s="2">
-        <v>10.604136361754588</v>
+        <v>9.45881645135891</v>
       </c>
     </row>
     <row r="145">
@@ -2555,7 +2555,7 @@
         <v>8.14</v>
       </c>
       <c r="E145" t="n" s="2">
-        <v>10.610713372388883</v>
+        <v>9.559025944959814</v>
       </c>
     </row>
     <row r="146">
@@ -2572,7 +2572,7 @@
         <v>8.12</v>
       </c>
       <c r="E146" t="n" s="2">
-        <v>10.627647494582378</v>
+        <v>9.57971468702644</v>
       </c>
     </row>
     <row r="147">
@@ -2589,7 +2589,7 @@
         <v>8.15</v>
       </c>
       <c r="E147" t="n" s="2">
-        <v>10.2483157513049</v>
+        <v>10.5759652993475</v>
       </c>
     </row>
     <row r="148">
@@ -2606,7 +2606,7 @@
         <v>8.17</v>
       </c>
       <c r="E148" t="n" s="2">
-        <v>10.69374956705076</v>
+        <v>9.58985595465962</v>
       </c>
     </row>
     <row r="149">
@@ -2623,7 +2623,7 @@
         <v>1.76</v>
       </c>
       <c r="E149" t="n" s="2">
-        <v>12.227871155795</v>
+        <v>9.015425045986094</v>
       </c>
     </row>
     <row r="150">
@@ -2640,7 +2640,7 @@
         <v>8.2</v>
       </c>
       <c r="E150" t="n" s="2">
-        <v>12.368814112345003</v>
+        <v>7.434115509907118</v>
       </c>
     </row>
     <row r="151">
@@ -2657,7 +2657,7 @@
         <v>8.12</v>
       </c>
       <c r="E151" t="n" s="2">
-        <v>9.97404339386277</v>
+        <v>8.19163028326565</v>
       </c>
     </row>
     <row r="152">
@@ -2674,7 +2674,7 @@
         <v>8.09</v>
       </c>
       <c r="E152" t="n" s="2">
-        <v>9.623997782354273</v>
+        <v>8.073739774328525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>